<commit_message>
Updated Trainign Set data
</commit_message>
<xml_diff>
--- a/SolubilityPS.xlsx
+++ b/SolubilityPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Himendra\Documents\Code\ConfocalImageAnalysis\CO2MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF821E22-4CD2-4962-98D5-80A63DD4D8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DCD725-CC19-4FDC-8F69-0AF1570CC691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="750" windowWidth="29010" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,69 +1686,147 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="1">
+        <v>373</v>
+      </c>
+      <c r="B77" s="3">
+        <v>0</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
+      <c r="A78" s="1">
+        <v>383</v>
+      </c>
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
+      <c r="C78" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
+      <c r="A79" s="1">
+        <v>393</v>
+      </c>
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
+      <c r="A80" s="1">
+        <v>403</v>
+      </c>
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+      <c r="C80" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
+      <c r="A81" s="1">
+        <v>413</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
+      <c r="A82" s="1">
+        <v>423</v>
+      </c>
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
+      <c r="C82" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="1">
+        <v>433</v>
+      </c>
+      <c r="B83" s="3">
+        <v>0</v>
+      </c>
+      <c r="C83" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+      <c r="A84" s="1">
+        <v>443</v>
+      </c>
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
+      <c r="C84" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="1">
+        <v>453</v>
+      </c>
+      <c r="B85" s="3">
+        <v>0</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
+      <c r="A86" s="1">
+        <v>463</v>
+      </c>
+      <c r="B86" s="3">
+        <v>0</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="1">
+        <v>473</v>
+      </c>
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
+      <c r="A88" s="1">
+        <v>483</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0</v>
+      </c>
+      <c r="C88" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
+      <c r="A89" s="1">
+        <v>493</v>
+      </c>
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+      <c r="C89" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>

</xml_diff>